<commit_message>
Created a word cloud for Module 1 bid list database
</commit_message>
<xml_diff>
--- a/5. Capstone Projects (Module 5)/Module 1/2025BidList.xlsx
+++ b/5. Capstone Projects (Module 5)/Module 1/2025BidList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imbuz\Documents\GitHub\Python4Everybody\5. Capstone Projects (Module 5)\Module 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E04E03-0B63-4C92-939D-B8241FCA3650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB222C9-AE14-4DDF-ADEB-5E7478342677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30510" yWindow="630" windowWidth="25095" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="projected_vacancies_2024_06_07_" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="270">
   <si>
     <t>Skill</t>
   </si>
@@ -195,9 +195,6 @@
     <t>(VANCOUVER) VANCOUVER                 BRITISH COLUMBIA (CG)</t>
   </si>
   <si>
-    <t>VANCOUVER, B.C.</t>
-  </si>
-  <si>
     <t>CAN</t>
   </si>
   <si>
@@ -390,9 +387,6 @@
   </si>
   <si>
     <t>The incumbent is the Commercial Diplomacy Officer in the Office of China Affairs, serving as the bureau-wide expert on commercial advocacy issues related to China, as well as a subject matter expert and coordinator on private sector commercial interests in China within the office.  The incumbent serves as EAPâ€™s primary action officer for messaging and outreach to the private sector, as well as engagement with U.S. and foreign private companies, industry associations, and other national and subnational stakeholder groups, including Embassy Beijing, the PRC Embassy in Washington, D.C., and the interagency and key policymakers and decisionmakers within the Department. The successful candidate should have experience both overseas and in Washington.  Previous China expertise is beneficial but not required.  This position is DETO-eligible. POCs â€“Hiring Manager: Ben LeRoy (LeRoyBA@state.gov); Bureau POC: Deputy Office Director Anny Vu (VuAL@state.gov).  In lieu of introductory emails, candidates must submit a personal statement to the lobbying POCs above.  This statement serves as a formal expression of interest; bidders do not need to submit additional materials or emails.  Submit lobbying documents through the 360CLC at http://exwebapps.state.sbu/CLC/.  EAP will not accept lobbying or endorsement emails outside of the CLC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>(LIMA) LIMA                     PERU</t>
@@ -583,9 +577,6 @@
     <t>(OTTAWA) OTTAWA                       CANADA</t>
   </si>
   <si>
-    <t>OTTAWA, ONTARIO</t>
-  </si>
-  <si>
     <t>Brennan</t>
   </si>
   <si>
@@ -593,9 +584,6 @@
   </si>
   <si>
     <t>(KOROR) KOROR,  REPUBLIC OF PALAU</t>
-  </si>
-  <si>
-    <t>KOROR, CAROLINE ISLAND</t>
   </si>
   <si>
     <t>PLW</t>
@@ -867,6 +855,24 @@
   </si>
   <si>
     <t>(Updated 07/2022) This is a CONSULTATIVE staffing position. Bidders should contact all the POCs listed. The incumbent is the sole Political/Economic Officer at U.S. Consulate General Nuevo Laredo. S/He reports directly to the Principal Officer and is reviewed by either the Political or Economic Minister Counselor in Mexico City. The incumbent manages the Pol/Econ Section, setting reporting and policy goals and managing a LE Pol/Econ Assistant and LE INL Outreach Coordinator. The incumbent coordinates efforts between other consulates and Embassy Mexico City to promote and advance U.S. political and economic interests in the border areas of Tamaulipas and Coahuila. Analyzes and reports on developments on all key political and economic bilateral issues in the district, including pivotal issues such as trade infrastructure, security, immigration, drug trafficking, energy, the manufacturing sector, political stability, conservation efforts, and labor and justice sector reforms. Serves as control officer for visits and collaborates with LES Public Diplomacy Assistant in drafting written materials and organizing public events for PD initiatives. Successful bidders need to demonstrate skills in these specific areas:  reporting officer skills, including drafting cables and briefing documents. POCs: Hiring Official: Deanna Kim KimDG@state.gov; Incumbent: Sun Lee LeeSJ2@state.gov; Consultative with Bureau: Jennifer Brown BrownJM3@state.gov (WHA/MEX). Please submit references through CLC: http://exwebapps.state.sbu/CLC.</t>
+  </si>
+  <si>
+    <t>KOROR -CAROLINE ISLAND</t>
+  </si>
+  <si>
+    <t>OTTAWA ONTARIO</t>
+  </si>
+  <si>
+    <t>VANCOUVER BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BRU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAH </t>
   </si>
 </sst>
 </file>
@@ -1771,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1943,7 @@
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1959,7 +1965,7 @@
         <v>17</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I5" s="2">
         <v>10</v>
@@ -1968,10 +1974,10 @@
         <v>45858</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1986,13 +1992,13 @@
         <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>22</v>
@@ -2007,10 +2013,10 @@
         <v>45869</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2025,13 +2031,13 @@
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>17</v>
@@ -2046,10 +2052,10 @@
         <v>45870</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2085,10 +2091,10 @@
         <v>45873</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2103,16 +2109,16 @@
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>180</v>
+        <v>264</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>23</v>
@@ -2124,10 +2130,10 @@
         <v>45884</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2142,16 +2148,16 @@
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>117</v>
+        <v>267</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>23</v>
@@ -2163,10 +2169,10 @@
         <v>45901</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2181,19 +2187,19 @@
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I11" s="2">
         <v>25</v>
@@ -2202,10 +2208,10 @@
         <v>45901</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2220,13 +2226,13 @@
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>17</v>
@@ -2241,10 +2247,10 @@
         <v>45912</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2259,16 +2265,16 @@
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>117</v>
+        <v>268</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>23</v>
@@ -2280,15 +2286,15 @@
         <v>45930</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2298,16 +2304,16 @@
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>23</v>
@@ -2319,10 +2325,10 @@
         <v>45937</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2376,19 +2382,19 @@
         <v>44</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I16" s="4">
         <v>0</v>
@@ -2397,10 +2403,10 @@
         <v>45837</v>
       </c>
       <c r="K16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2415,13 +2421,13 @@
         <v>44</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>22</v>
@@ -2436,15 +2442,15 @@
         <v>45839</v>
       </c>
       <c r="K17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2454,13 +2460,13 @@
         <v>44</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>22</v>
@@ -2478,12 +2484,12 @@
         <v>18</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2493,19 +2499,19 @@
         <v>44</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="I19" s="4">
         <v>25</v>
@@ -2514,15 +2520,15 @@
         <v>45841</v>
       </c>
       <c r="K19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2532,13 +2538,13 @@
         <v>44</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>22</v>
@@ -2553,10 +2559,10 @@
         <v>45865</v>
       </c>
       <c r="K20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2571,13 +2577,13 @@
         <v>44</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>22</v>
@@ -2592,10 +2598,10 @@
         <v>45871</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2610,13 +2616,13 @@
         <v>44</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>22</v>
@@ -2631,15 +2637,15 @@
         <v>45874</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2649,13 +2655,13 @@
         <v>44</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>22</v>
@@ -2670,10 +2676,10 @@
         <v>45876</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2688,13 +2694,13 @@
         <v>44</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>22</v>
@@ -2709,10 +2715,10 @@
         <v>45879</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2727,13 +2733,13 @@
         <v>44</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>22</v>
@@ -2748,10 +2754,10 @@
         <v>45884</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2766,13 +2772,13 @@
         <v>44</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>22</v>
@@ -2787,10 +2793,10 @@
         <v>45888</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2805,13 +2811,13 @@
         <v>44</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>22</v>
@@ -2826,10 +2832,10 @@
         <v>45909</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2844,13 +2850,13 @@
         <v>44</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>22</v>
@@ -2865,15 +2871,15 @@
         <v>45918</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2883,13 +2889,13 @@
         <v>44</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>22</v>
@@ -2904,10 +2910,10 @@
         <v>45958</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2964,10 +2970,10 @@
         <v>51</v>
       </c>
       <c r="E31" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>22</v>
@@ -2982,10 +2988,10 @@
         <v>45827</v>
       </c>
       <c r="K31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L31" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3000,13 +3006,13 @@
         <v>29</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>17</v>
@@ -3021,10 +3027,10 @@
         <v>45845</v>
       </c>
       <c r="K32" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L32" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3039,13 +3045,13 @@
         <v>29</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>40</v>
@@ -3060,10 +3066,10 @@
         <v>45848</v>
       </c>
       <c r="K33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L33" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3078,13 +3084,13 @@
         <v>29</v>
       </c>
       <c r="D34" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>17</v>
@@ -3099,15 +3105,15 @@
         <v>45853</v>
       </c>
       <c r="K34" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="L34" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3117,13 +3123,13 @@
         <v>29</v>
       </c>
       <c r="D35" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>106</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>17</v>
@@ -3138,10 +3144,10 @@
         <v>45867</v>
       </c>
       <c r="K35" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="L35" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3156,13 +3162,13 @@
         <v>29</v>
       </c>
       <c r="D36" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>17</v>
@@ -3177,10 +3183,10 @@
         <v>45868</v>
       </c>
       <c r="K36" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L36" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="L36" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3195,13 +3201,13 @@
         <v>29</v>
       </c>
       <c r="D37" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>17</v>
@@ -3216,15 +3222,15 @@
         <v>45870</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B38" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3234,13 +3240,13 @@
         <v>29</v>
       </c>
       <c r="D38" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>126</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>17</v>
@@ -3255,10 +3261,10 @@
         <v>45870</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3273,13 +3279,13 @@
         <v>29</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>17</v>
@@ -3294,15 +3300,15 @@
         <v>45870</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B40" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3333,15 +3339,15 @@
         <v>45871</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B41" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3351,13 +3357,13 @@
         <v>29</v>
       </c>
       <c r="D41" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>17</v>
@@ -3372,15 +3378,15 @@
         <v>45873</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B42" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3411,10 +3417,10 @@
         <v>45873</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3429,13 +3435,13 @@
         <v>29</v>
       </c>
       <c r="D43" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>17</v>
@@ -3450,10 +3456,10 @@
         <v>45881</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3468,13 +3474,13 @@
         <v>29</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>17</v>
@@ -3489,10 +3495,10 @@
         <v>45881</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3507,13 +3513,13 @@
         <v>29</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>176</v>
+        <v>265</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>22</v>
@@ -3528,10 +3534,10 @@
         <v>45884</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3546,16 +3552,16 @@
         <v>29</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>33</v>
@@ -3567,10 +3573,10 @@
         <v>45886</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3585,13 +3591,13 @@
         <v>29</v>
       </c>
       <c r="D47" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>17</v>
@@ -3606,15 +3612,15 @@
         <v>45894</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B48" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3624,13 +3630,13 @@
         <v>29</v>
       </c>
       <c r="D48" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>17</v>
@@ -3645,10 +3651,10 @@
         <v>45897</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3663,13 +3669,13 @@
         <v>29</v>
       </c>
       <c r="D49" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="F49" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>17</v>
@@ -3684,7 +3690,7 @@
         <v>45901</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="L49" s="6" t="s">
         <v>23</v>
@@ -3702,13 +3708,13 @@
         <v>29</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>17</v>
@@ -3723,15 +3729,15 @@
         <v>45901</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3741,13 +3747,13 @@
         <v>29</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>22</v>
@@ -3762,10 +3768,10 @@
         <v>45903</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3780,13 +3786,13 @@
         <v>29</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>117</v>
+        <v>269</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>17</v>
@@ -3801,15 +3807,15 @@
         <v>45908</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B53" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3819,13 +3825,13 @@
         <v>29</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>17</v>
@@ -3840,15 +3846,15 @@
         <v>45923</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3858,13 +3864,13 @@
         <v>29</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>17</v>
@@ -3879,10 +3885,10 @@
         <v>45931</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="L54" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3897,13 +3903,13 @@
         <v>29</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>17</v>
@@ -3918,10 +3924,10 @@
         <v>45931</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3936,16 +3942,16 @@
         <v>29</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>23</v>
@@ -3957,10 +3963,10 @@
         <v>45931</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="57" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3975,13 +3981,13 @@
         <v>29</v>
       </c>
       <c r="D57" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>17</v>
@@ -3996,10 +4002,10 @@
         <v>45954</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4014,16 +4020,16 @@
         <v>29</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>33</v>
@@ -4035,10 +4041,10 @@
         <v>46127</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>